<commit_message>
microcontroller added and started writing about finans
</commit_message>
<xml_diff>
--- a/BOM_totaal.xlsx
+++ b/BOM_totaal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B36704-28BC-48DF-B5DC-25413E036557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB2BA3A-F253-439F-ACCE-46D08B535D22}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7890" yWindow="2250" windowWidth="18630" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="152">
   <si>
     <t>Part No.</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t>TLHG44K1L2</t>
+  </si>
+  <si>
+    <t>Prijs tot</t>
+  </si>
+  <si>
+    <t>Tot:</t>
   </si>
 </sst>
 </file>
@@ -884,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,11 +904,12 @@
     <col min="4" max="4" width="10.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="220.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="7" width="10.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="220.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -921,10 +928,12 @@
       <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -936,8 +945,9 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
-    </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T1" s="4"/>
+    </row>
+    <row r="2" spans="1:20" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -954,10 +964,13 @@
       <c r="F2" s="8">
         <v>4.95</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="8">
+        <f>E2*F2</f>
+        <v>9.9</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -969,8 +982,9 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -979,8 +993,11 @@
       <c r="F3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="8" t="e">
+        <f t="shared" ref="G3:G42" si="0">E3*F3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" s="5"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -992,8 +1009,9 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1010,10 +1028,13 @@
       <c r="F4" s="8">
         <v>2.17</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>4.34</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1025,8 +1046,9 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" spans="1:20" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -1045,10 +1067,13 @@
       <c r="F5" s="8">
         <v>1.99</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="8">
+        <f t="shared" si="0"/>
+        <v>1.99</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1060,8 +1085,9 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -1078,10 +1104,13 @@
       <c r="F6" s="8">
         <v>0.6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1093,8 +1122,9 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1110,11 +1140,15 @@
       <c r="F7" s="8">
         <v>0.54</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
@@ -1130,11 +1164,15 @@
       <c r="F8" s="8">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>78</v>
       </c>
@@ -1147,11 +1185,15 @@
       <c r="F9" s="8">
         <v>1.89</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>1.89</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
@@ -1170,11 +1212,15 @@
       <c r="F10" s="8">
         <v>0.33</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>81</v>
       </c>
@@ -1187,11 +1233,15 @@
       <c r="F11" s="8">
         <v>0.38</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>33</v>
       </c>
@@ -1210,11 +1260,15 @@
       <c r="F12" s="8">
         <v>6.26</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="8">
+        <f t="shared" si="0"/>
+        <v>6.26</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
@@ -1233,11 +1287,15 @@
       <c r="F13" s="8">
         <v>10.17</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="8">
+        <f t="shared" si="0"/>
+        <v>10.17</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>37</v>
       </c>
@@ -1253,11 +1311,15 @@
       <c r="F14" s="8">
         <v>27.04</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="8">
+        <f t="shared" si="0"/>
+        <v>27.04</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>53</v>
       </c>
@@ -1276,11 +1338,15 @@
       <c r="F15" s="8">
         <v>0.35099999999999998</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="8">
+        <f t="shared" si="0"/>
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>93</v>
       </c>
@@ -1296,11 +1362,15 @@
       <c r="F16" s="8">
         <v>3.06</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="8">
+        <f t="shared" si="0"/>
+        <v>3.06</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>86</v>
       </c>
@@ -1313,11 +1383,15 @@
       <c r="F17" s="8">
         <v>0.45900000000000002</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="8">
+        <f t="shared" si="0"/>
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>61</v>
       </c>
@@ -1336,11 +1410,15 @@
       <c r="F18" s="8">
         <v>0.42</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="8">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>76</v>
       </c>
@@ -1359,11 +1437,15 @@
       <c r="F19" s="8">
         <v>0.29699999999999999</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="8">
+        <f t="shared" si="0"/>
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>95</v>
       </c>
@@ -1379,11 +1461,15 @@
       <c r="F20" s="8">
         <v>0.92</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="8">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>96</v>
       </c>
@@ -1399,11 +1485,15 @@
       <c r="F21" s="8">
         <v>0.52</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="8">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>145</v>
       </c>
@@ -1416,18 +1506,26 @@
       <c r="F22" s="8">
         <v>0.32</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="8">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>94</v>
       </c>
@@ -1446,11 +1544,15 @@
       <c r="F24" s="8">
         <v>0.09</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="8">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>330</v>
       </c>
@@ -1463,11 +1565,15 @@
       <c r="F25" s="8">
         <v>0.09</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>680</v>
       </c>
@@ -1480,11 +1586,15 @@
       <c r="F26" s="8">
         <v>0.09</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="8">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>100</v>
       </c>
@@ -1497,11 +1607,15 @@
       <c r="F27" s="8">
         <v>0.09</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="8">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>103</v>
       </c>
@@ -1514,11 +1628,15 @@
       <c r="F28" s="8">
         <v>0.09</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>104</v>
       </c>
@@ -1531,11 +1649,15 @@
       <c r="F29" s="8">
         <v>0.09</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="8">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>71</v>
       </c>
@@ -1551,11 +1673,15 @@
       <c r="F30" s="8">
         <v>0.09</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="8">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>102</v>
       </c>
@@ -1568,11 +1694,15 @@
       <c r="F31" s="8">
         <v>0.09</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="8">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>101</v>
       </c>
@@ -1585,11 +1715,15 @@
       <c r="F32" s="8">
         <v>0.09</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="8">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>72</v>
       </c>
@@ -1605,11 +1739,15 @@
       <c r="F33" s="8">
         <v>0.09</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="8">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>105</v>
       </c>
@@ -1622,11 +1760,15 @@
       <c r="F34" s="8">
         <v>0.09</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>106</v>
       </c>
@@ -1645,11 +1787,15 @@
       <c r="F35" s="8">
         <v>0.23</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="8">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>111</v>
       </c>
@@ -1665,11 +1811,15 @@
       <c r="F36" s="8">
         <v>0.22</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="8">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>115</v>
       </c>
@@ -1685,11 +1835,15 @@
       <c r="F37" s="8">
         <v>0.24</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="8">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>144</v>
       </c>
@@ -1708,11 +1862,15 @@
       <c r="F38" s="8">
         <v>0.35</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G38" s="8">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>66</v>
       </c>
@@ -1728,11 +1886,15 @@
       <c r="F39" s="8">
         <v>0.26100000000000001</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G39" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3050000000000002</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>65</v>
       </c>
@@ -1748,11 +1910,15 @@
       <c r="F40" s="8">
         <v>0.29699999999999999</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="8">
+        <f t="shared" si="0"/>
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="H40" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>64</v>
       </c>
@@ -1768,11 +1934,15 @@
       <c r="F41" s="8">
         <v>0.36899999999999999</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="8">
+        <f t="shared" si="0"/>
+        <v>1.107</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>63</v>
       </c>
@@ -1788,11 +1958,15 @@
       <c r="F42" s="8">
         <v>0.27900000000000003</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="8">
+        <f t="shared" si="0"/>
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>119</v>
       </c>
@@ -1808,50 +1982,63 @@
       <c r="F43" s="8">
         <v>0.76</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="8">
+        <f>E43*F43</f>
+        <v>0.76</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F45" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G45" s="8">
+        <f>SUM(G4:G44)</f>
+        <v>71.704000000000022</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{BE201204-4D76-4D99-A136-97852DAF4D35}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
-    <hyperlink ref="G7" r:id="rId4" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
-    <hyperlink ref="G8" r:id="rId5" xr:uid="{96DFE09D-FE4D-4147-A8CE-602A5DDFBFA7}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{682E6110-B477-43CD-9147-49CEB11861DF}"/>
-    <hyperlink ref="G15" r:id="rId7" xr:uid="{426BD05D-D8EF-43D7-A582-AC4F8E600E5F}"/>
-    <hyperlink ref="G13" r:id="rId8" xr:uid="{6E401E59-3667-4D7F-ABA4-4D7A0A7A91E1}"/>
-    <hyperlink ref="G14" r:id="rId9" xr:uid="{340F4965-1516-4699-A1F1-2E724698C5D3}"/>
-    <hyperlink ref="G12" r:id="rId10" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
-    <hyperlink ref="G18" r:id="rId11" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
-    <hyperlink ref="G19" r:id="rId12" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
-    <hyperlink ref="G41" r:id="rId13" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
-    <hyperlink ref="G24" r:id="rId14" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
-    <hyperlink ref="G30" r:id="rId15" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
-    <hyperlink ref="G33" r:id="rId16" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
-    <hyperlink ref="G9" r:id="rId17" xr:uid="{092811F2-67AA-404B-8561-69F45A6D17C5}"/>
-    <hyperlink ref="G11" r:id="rId18" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
-    <hyperlink ref="G16" r:id="rId19" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
-    <hyperlink ref="G17" r:id="rId20" xr:uid="{B022C6F2-66BF-4E7D-AE9A-E110C3B9196E}"/>
-    <hyperlink ref="G10" r:id="rId21" xr:uid="{5D93DF65-24C6-4E51-A510-3921BED8E11B}"/>
-    <hyperlink ref="G21" r:id="rId22" xr:uid="{189818F7-AA8F-4727-9185-CEA50EF2695D}"/>
-    <hyperlink ref="G20" r:id="rId23" xr:uid="{53AA5B85-A885-4355-9507-7D4FAD9E6E7A}"/>
-    <hyperlink ref="G35" r:id="rId24" xr:uid="{258B17CA-7BC0-49B1-9646-4348361BA522}"/>
-    <hyperlink ref="G36" r:id="rId25" xr:uid="{850A7ECD-14D3-4AE8-9F8D-82209F865128}"/>
-    <hyperlink ref="G37" r:id="rId26" xr:uid="{15EB3110-02A8-4DE6-85CA-C6ADD5F5B2B7}"/>
-    <hyperlink ref="G43" r:id="rId27" xr:uid="{4098B0A1-B48A-4B0E-B2AA-660FD27291C7}"/>
-    <hyperlink ref="G28" r:id="rId28" xr:uid="{927B8ABD-8118-4683-A15B-0391A64D25B0}"/>
-    <hyperlink ref="G32" r:id="rId29" xr:uid="{3D6C7538-7627-4B9D-8B3D-D15061B23A16}"/>
-    <hyperlink ref="G26" r:id="rId30" xr:uid="{279BEC83-2CA6-41EF-9AE3-B022003183BD}"/>
-    <hyperlink ref="G25" r:id="rId31" xr:uid="{B87D843C-6406-4920-A163-0FC7D8E02A21}"/>
-    <hyperlink ref="G31" r:id="rId32" xr:uid="{A6F2E23E-2ECA-4D71-89DA-48017F96F806}"/>
-    <hyperlink ref="G29" r:id="rId33" xr:uid="{3DDD5F0B-8AB4-49FE-94B2-EB4BFC2F6341}"/>
-    <hyperlink ref="G27" r:id="rId34" xr:uid="{5DC8BB42-9D99-4E5B-8243-EDE54EB8887E}"/>
-    <hyperlink ref="G34" r:id="rId35" xr:uid="{32C0F45F-109A-4F6D-A45D-7B21ECE165A6}"/>
-    <hyperlink ref="G39" r:id="rId36" xr:uid="{A9F14920-0F15-4721-A0F0-758F592CC933}"/>
-    <hyperlink ref="G22" r:id="rId37" xr:uid="{2D9C6DEC-9229-4AAB-A2FA-39A71B7475D3}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{BE201204-4D76-4D99-A136-97852DAF4D35}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
+    <hyperlink ref="H8" r:id="rId5" xr:uid="{96DFE09D-FE4D-4147-A8CE-602A5DDFBFA7}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{682E6110-B477-43CD-9147-49CEB11861DF}"/>
+    <hyperlink ref="H15" r:id="rId7" xr:uid="{426BD05D-D8EF-43D7-A582-AC4F8E600E5F}"/>
+    <hyperlink ref="H13" r:id="rId8" xr:uid="{6E401E59-3667-4D7F-ABA4-4D7A0A7A91E1}"/>
+    <hyperlink ref="H14" r:id="rId9" xr:uid="{340F4965-1516-4699-A1F1-2E724698C5D3}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
+    <hyperlink ref="H18" r:id="rId11" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
+    <hyperlink ref="H19" r:id="rId12" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
+    <hyperlink ref="H41" r:id="rId13" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
+    <hyperlink ref="H24" r:id="rId14" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
+    <hyperlink ref="H30" r:id="rId15" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
+    <hyperlink ref="H33" r:id="rId16" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
+    <hyperlink ref="H9" r:id="rId17" xr:uid="{092811F2-67AA-404B-8561-69F45A6D17C5}"/>
+    <hyperlink ref="H11" r:id="rId18" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
+    <hyperlink ref="H16" r:id="rId19" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
+    <hyperlink ref="H17" r:id="rId20" xr:uid="{B022C6F2-66BF-4E7D-AE9A-E110C3B9196E}"/>
+    <hyperlink ref="H10" r:id="rId21" xr:uid="{5D93DF65-24C6-4E51-A510-3921BED8E11B}"/>
+    <hyperlink ref="H21" r:id="rId22" xr:uid="{189818F7-AA8F-4727-9185-CEA50EF2695D}"/>
+    <hyperlink ref="H20" r:id="rId23" xr:uid="{53AA5B85-A885-4355-9507-7D4FAD9E6E7A}"/>
+    <hyperlink ref="H35" r:id="rId24" xr:uid="{258B17CA-7BC0-49B1-9646-4348361BA522}"/>
+    <hyperlink ref="H36" r:id="rId25" xr:uid="{850A7ECD-14D3-4AE8-9F8D-82209F865128}"/>
+    <hyperlink ref="H37" r:id="rId26" xr:uid="{15EB3110-02A8-4DE6-85CA-C6ADD5F5B2B7}"/>
+    <hyperlink ref="H43" r:id="rId27" xr:uid="{4098B0A1-B48A-4B0E-B2AA-660FD27291C7}"/>
+    <hyperlink ref="H28" r:id="rId28" xr:uid="{927B8ABD-8118-4683-A15B-0391A64D25B0}"/>
+    <hyperlink ref="H32" r:id="rId29" xr:uid="{3D6C7538-7627-4B9D-8B3D-D15061B23A16}"/>
+    <hyperlink ref="H26" r:id="rId30" xr:uid="{279BEC83-2CA6-41EF-9AE3-B022003183BD}"/>
+    <hyperlink ref="H25" r:id="rId31" xr:uid="{B87D843C-6406-4920-A163-0FC7D8E02A21}"/>
+    <hyperlink ref="H31" r:id="rId32" xr:uid="{A6F2E23E-2ECA-4D71-89DA-48017F96F806}"/>
+    <hyperlink ref="H29" r:id="rId33" xr:uid="{3DDD5F0B-8AB4-49FE-94B2-EB4BFC2F6341}"/>
+    <hyperlink ref="H27" r:id="rId34" xr:uid="{5DC8BB42-9D99-4E5B-8243-EDE54EB8887E}"/>
+    <hyperlink ref="H34" r:id="rId35" xr:uid="{32C0F45F-109A-4F6D-A45D-7B21ECE165A6}"/>
+    <hyperlink ref="H39" r:id="rId36" xr:uid="{A9F14920-0F15-4721-A0F0-758F592CC933}"/>
+    <hyperlink ref="H22" r:id="rId37" xr:uid="{2D9C6DEC-9229-4AAB-A2FA-39A71B7475D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId38"/>

</xml_diff>